<commit_message>
update sample and main
</commit_message>
<xml_diff>
--- a/app/static/sample.xlsx
+++ b/app/static/sample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="16560" activeTab="1"/>
+    <workbookView windowHeight="17160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="10">
   <si>
     <t>uuid</t>
   </si>
@@ -1093,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E4"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
@@ -1186,254 +1186,518 @@
       <c r="G4" s="25"/>
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:7">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="A5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="18">
+        <v>45508.375</v>
+      </c>
+      <c r="D5" s="18">
+        <v>45508.375</v>
+      </c>
+      <c r="E5" s="18">
+        <v>45508.7083333333</v>
+      </c>
       <c r="F5" s="22"/>
       <c r="G5" s="25"/>
     </row>
     <row r="6" ht="17.25" customHeight="1" spans="1:7">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="18">
+        <v>45509.375</v>
+      </c>
+      <c r="D6" s="18">
+        <v>45509.375</v>
+      </c>
+      <c r="E6" s="18">
+        <v>45509.7083333333</v>
+      </c>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
     </row>
     <row r="7" ht="17.25" customHeight="1" spans="1:7">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="A7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="18">
+        <v>45510.375</v>
+      </c>
+      <c r="D7" s="18">
+        <v>45510.375</v>
+      </c>
+      <c r="E7" s="18">
+        <v>45510.7083333333</v>
+      </c>
       <c r="F7" s="22"/>
       <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="18">
+        <v>45511.375</v>
+      </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="F8" s="22"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="18">
+        <v>45512.375</v>
+      </c>
+      <c r="D9" s="18">
+        <v>45512.375</v>
+      </c>
+      <c r="E9" s="18">
+        <v>45512.7083333333</v>
+      </c>
       <c r="F9" s="22"/>
       <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="A10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="18">
+        <v>45513.375</v>
+      </c>
+      <c r="D10" s="18">
+        <v>45513.375</v>
+      </c>
+      <c r="E10" s="18">
+        <v>45513.7083333333</v>
+      </c>
       <c r="F10" s="22"/>
       <c r="G10" s="25"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="A11" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="18">
+        <v>45514.375</v>
+      </c>
+      <c r="D11" s="18">
+        <v>45514.375</v>
+      </c>
+      <c r="E11" s="18">
+        <v>45514.7083333333</v>
+      </c>
       <c r="F11" s="22"/>
       <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="18">
+        <v>45515.375</v>
+      </c>
+      <c r="D12" s="18">
+        <v>45515.375</v>
+      </c>
+      <c r="E12" s="18">
+        <v>45515.7083333333</v>
+      </c>
       <c r="F12" s="22"/>
       <c r="G12" s="25"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="A13" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18">
+        <v>45516.375</v>
+      </c>
+      <c r="D13" s="18">
+        <v>45516.375</v>
+      </c>
+      <c r="E13" s="18">
+        <v>45516.7083333333</v>
+      </c>
       <c r="F13" s="22"/>
       <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="16"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="A14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="18">
+        <v>45517.375</v>
+      </c>
+      <c r="D14" s="18">
+        <v>45517.375</v>
+      </c>
+      <c r="E14" s="18">
+        <v>45517.7083333333</v>
+      </c>
       <c r="F14" s="22"/>
       <c r="G14" s="25"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="A15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="18">
+        <v>45518.375</v>
+      </c>
+      <c r="D15" s="18">
+        <v>45518.375</v>
+      </c>
+      <c r="E15" s="18">
+        <v>45518.7083333333</v>
+      </c>
       <c r="F15" s="22"/>
       <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="18">
+        <v>45519.375</v>
+      </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="A17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="18">
+        <v>45520.375</v>
+      </c>
+      <c r="D17" s="18">
+        <v>45520.375</v>
+      </c>
+      <c r="E17" s="18">
+        <v>45520.7083333333</v>
+      </c>
       <c r="F17" s="22"/>
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="A18" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="18">
+        <v>45521.375</v>
+      </c>
+      <c r="D18" s="18">
+        <v>45521.375</v>
+      </c>
+      <c r="E18" s="18">
+        <v>45521.7083333333</v>
+      </c>
       <c r="F18" s="22"/>
       <c r="G18" s="25"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="A19" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="18">
+        <v>45522.375</v>
+      </c>
+      <c r="D19" s="18">
+        <v>45522.375</v>
+      </c>
+      <c r="E19" s="18">
+        <v>45522.7083333333</v>
+      </c>
       <c r="F19" s="22"/>
       <c r="G19" s="25"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
+      <c r="A20" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="18">
+        <v>45523.375</v>
+      </c>
+      <c r="D20" s="18">
+        <v>45523.375</v>
+      </c>
+      <c r="E20" s="18">
+        <v>45523.7083333333</v>
+      </c>
       <c r="F20" s="22"/>
       <c r="G20" s="25"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="A21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="18">
+        <v>45524.375</v>
+      </c>
+      <c r="D21" s="18">
+        <v>45524.375</v>
+      </c>
+      <c r="E21" s="18">
+        <v>45524.7083333333</v>
+      </c>
       <c r="F21" s="22"/>
       <c r="G21" s="25"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="18">
+        <v>45525.375</v>
+      </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="22"/>
       <c r="G22" s="25"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
+      <c r="A23" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="18">
+        <v>45526.375</v>
+      </c>
+      <c r="D23" s="18">
+        <v>45526.375</v>
+      </c>
+      <c r="E23" s="18">
+        <v>45526.7083333333</v>
+      </c>
       <c r="F23" s="22"/>
       <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="A24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="18">
+        <v>45527.375</v>
+      </c>
+      <c r="D24" s="18">
+        <v>45527.375</v>
+      </c>
+      <c r="E24" s="18">
+        <v>45527.7083333333</v>
+      </c>
       <c r="F24" s="22"/>
       <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="A25" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="18">
+        <v>45528.375</v>
+      </c>
+      <c r="D25" s="18">
+        <v>45528.375</v>
+      </c>
+      <c r="E25" s="18">
+        <v>45528.7083333333</v>
+      </c>
       <c r="F25" s="22"/>
       <c r="G25" s="25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="A26" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="18">
+        <v>45529.375</v>
+      </c>
+      <c r="D26" s="18">
+        <v>45529.375</v>
+      </c>
+      <c r="E26" s="18">
+        <v>45529.7083333333</v>
+      </c>
       <c r="F26" s="22"/>
       <c r="G26" s="25"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="16"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
+      <c r="A27" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="18">
+        <v>45530.375</v>
+      </c>
+      <c r="D27" s="18">
+        <v>45530.375</v>
+      </c>
+      <c r="E27" s="18">
+        <v>45530.7083333333</v>
+      </c>
       <c r="F27" s="22"/>
       <c r="G27" s="25"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
+      <c r="A28" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="18">
+        <v>45531.375</v>
+      </c>
+      <c r="D28" s="18">
+        <v>45531.375</v>
+      </c>
+      <c r="E28" s="18">
+        <v>45531.7083333333</v>
+      </c>
       <c r="F28" s="22"/>
       <c r="G28" s="25"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="16"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="18">
+        <v>45532.375</v>
+      </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="22"/>
       <c r="G29" s="25"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="16"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
+      <c r="A30" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="18">
+        <v>45533.375</v>
+      </c>
+      <c r="D30" s="18">
+        <v>45533.375</v>
+      </c>
+      <c r="E30" s="18">
+        <v>45533.7083333333</v>
+      </c>
       <c r="F30" s="22"/>
       <c r="G30" s="25"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="16"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="A31" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="18">
+        <v>45534.375</v>
+      </c>
+      <c r="D31" s="18">
+        <v>45534.375</v>
+      </c>
+      <c r="E31" s="18">
+        <v>45534.7083333333</v>
+      </c>
       <c r="F31" s="22"/>
       <c r="G31" s="25"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
+      <c r="A32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="18">
+        <v>45535.375</v>
+      </c>
+      <c r="D32" s="18">
+        <v>45535.375</v>
+      </c>
+      <c r="E32" s="18">
+        <v>45535.7083333333</v>
+      </c>
       <c r="F32" s="22"/>
       <c r="G32" s="25"/>
     </row>
@@ -2296,7 +2560,7 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>